<commit_message>
Fix for new ifc
</commit_message>
<xml_diff>
--- a/Construction_Isolants_classified.xlsx
+++ b/Construction_Isolants_classified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@\@CESI\Stage CESI\Code\Rsimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13D76FB-B0FB-4D02-9830-57D1FD37C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327BB308-183E-4983-8E89-52E293C9B4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Isolants</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Nom_Matériau</t>
+  </si>
+  <si>
+    <t>Blocs béton manufacturés</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,6 +468,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>